<commit_message>
Revised the notebook, uploaded the experiment data, and adding the output.txt
</commit_message>
<xml_diff>
--- a/data/processed/den/Exp_2bola.xlsx
+++ b/data/processed/den/Exp_2bola.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Project\Python\ml4spec2linconf\data\processed\den\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139008B3-B2E2-49BE-ACAF-95B6A8E50D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FA9F76-CA48-41FB-B367-31A9C2DA20BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0D65F594-1415-48AA-BB3B-CFD171DDB51E}"/>
   </bookViews>
@@ -55,8 +55,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,8 +374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3C07B8-76E4-4D0F-8C0A-95441F3C4BD5}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,27 +384,27 @@
       <c r="A1">
         <v>513</v>
       </c>
-      <c r="B1">
-        <v>10.27</v>
+      <c r="B1" s="1">
+        <v>1.027E-14</v>
       </c>
       <c r="C1">
         <v>537</v>
       </c>
-      <c r="D1">
-        <v>8.6</v>
+      <c r="D1" s="1">
+        <v>8.5999999999999993E-15</v>
       </c>
       <c r="E1">
         <v>643.29999999999995</v>
       </c>
       <c r="F1">
         <f>(H1-D1)/2+D1</f>
-        <v>35.29</v>
+        <v>3.5290000000000007E-14</v>
       </c>
       <c r="G1">
         <v>868.88</v>
       </c>
-      <c r="H1">
-        <v>61.98</v>
+      <c r="H1" s="1">
+        <v>6.1980000000000004E-14</v>
       </c>
       <c r="I1">
         <v>723.3</v>
@@ -450,27 +451,27 @@
       <c r="A2">
         <v>507</v>
       </c>
-      <c r="B2">
-        <v>11.11</v>
+      <c r="B2" s="1">
+        <v>1.1109999999999999E-14</v>
       </c>
       <c r="C2">
         <v>531.11</v>
       </c>
-      <c r="D2">
-        <v>8.33</v>
+      <c r="D2" s="1">
+        <v>8.3299999999999993E-15</v>
       </c>
       <c r="E2">
         <v>634</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F4" si="0">(H2-D2)/2+D2</f>
-        <v>28.7485</v>
+        <v>2.8748499999999996E-14</v>
       </c>
       <c r="G2">
         <v>681.1</v>
       </c>
-      <c r="H2">
-        <v>49.167000000000002</v>
+      <c r="H2" s="1">
+        <v>4.9166999999999998E-14</v>
       </c>
       <c r="I2">
         <v>721</v>
@@ -517,27 +518,27 @@
       <c r="A3">
         <v>563</v>
       </c>
-      <c r="B3">
-        <v>15</v>
+      <c r="B3" s="1">
+        <v>1.4999999999999999E-14</v>
       </c>
       <c r="C3">
         <v>603</v>
       </c>
-      <c r="D3">
-        <v>14.4</v>
+      <c r="D3" s="1">
+        <v>1.44E-14</v>
       </c>
       <c r="E3">
         <v>645.6</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>20.18</v>
+        <v>2.0180000000000002E-14</v>
       </c>
       <c r="G3">
         <v>680</v>
       </c>
-      <c r="H3">
-        <v>25.96</v>
+      <c r="H3" s="1">
+        <v>2.5960000000000001E-14</v>
       </c>
       <c r="I3">
         <v>707.6</v>
@@ -584,27 +585,27 @@
       <c r="A4">
         <v>506</v>
       </c>
-      <c r="B4">
-        <v>12.8</v>
+      <c r="B4" s="1">
+        <v>1.28E-14</v>
       </c>
       <c r="C4">
         <v>533.69000000000005</v>
       </c>
-      <c r="D4">
-        <v>9.23</v>
+      <c r="D4" s="1">
+        <v>9.2300000000000005E-15</v>
       </c>
       <c r="E4">
         <v>592</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>26.245000000000001</v>
+        <v>2.6244999999999999E-14</v>
       </c>
       <c r="G4">
         <v>638</v>
       </c>
-      <c r="H4">
-        <v>43.26</v>
+      <c r="H4" s="1">
+        <v>4.3259999999999997E-14</v>
       </c>
       <c r="I4">
         <v>706</v>

</xml_diff>